<commit_message>
FB70 and FB03 changes moving to github
</commit_message>
<xml_diff>
--- a/Tests/Resource/invoice.xlsx
+++ b/Tests/Resource/invoice.xlsx
@@ -450,7 +450,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -533,7 +533,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20.02.2024</t>
+          <t>22.02.2024</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -555,12 +555,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Document 1800000424 was posted in company code 3000</t>
+          <t>Document 1800000442 was posted in company code 3000</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1800000424</t>
+          <t>1800000442</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -573,10 +573,98 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CMS0000043</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>22.02.2024</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Robo Test1</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>40001</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="n">
+        <v>329</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Document 1800000443 was posted in company code 3000</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1800000443</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>2024</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CMS0000043</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>22.02.2024</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Robo Test2</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>40001</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="G4" t="n">
+        <v>329</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Document 1800000444 was posted in company code 3000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1800000444</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>2024</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>

</xml_diff>

<commit_message>
updated fb transaction files
</commit_message>
<xml_diff>
--- a/Tests/Resource/invoice.xlsx
+++ b/Tests/Resource/invoice.xlsx
@@ -1,33 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\Symphony_Testing\repo.symphony_testing\Tests\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B809A5A-64B8-435D-9C71-5EEFF98512BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INPUT" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="INPUT" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+  <si>
+    <t xml:space="preserve"> Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Invoice Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amount</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>G/L Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Amount in doc. curr.</t>
+  </si>
+  <si>
+    <t>Cost Center</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Company Code</t>
+  </si>
+  <si>
+    <t>Fiscal Year</t>
+  </si>
+  <si>
+    <t>CMS0000043</t>
+  </si>
+  <si>
+    <t>Robo Test</t>
+  </si>
+  <si>
+    <t>Document 1800000445 was posted in company code 3000</t>
+  </si>
+  <si>
+    <t>1800000445</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>Robo Test1</t>
+  </si>
+  <si>
+    <t>Document 1800000446 was posted in company code 3000</t>
+  </si>
+  <si>
+    <t>1800000446</t>
+  </si>
+  <si>
+    <t>Robo Test2</t>
+  </si>
+  <si>
+    <t>Document 1800000447 was posted in company code 3000</t>
+  </si>
+  <si>
+    <t>1800000447</t>
+  </si>
+  <si>
+    <t>23.02.2024</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,83 +125,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -442,241 +462,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="25.7109375" customWidth="1" min="2" max="2"/>
-    <col width="15.42578125" customWidth="1" min="3" max="3"/>
-    <col width="15.7109375" customWidth="1" min="4" max="4"/>
-    <col width="15.5703125" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
-    <col width="17.7109375" customWidth="1" min="7" max="7"/>
-    <col width="54.5703125" customWidth="1" min="8" max="8"/>
-    <col width="26.5703125" customWidth="1" min="9" max="9"/>
-    <col width="27.42578125" customWidth="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" min="11" max="11"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="54.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Customer</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Invoice Date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Amount</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>G/L Account</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Amount in doc. curr.</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Cost Center</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Output</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Document</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Company Code</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Fiscal Year</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>CMS0000043</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>22.02.2024</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
         <v>1000</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Robo Test</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
         <v>40001</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>1000</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>329</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Document 1800000442 was posted in company code 3000</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1800000442</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2">
         <v>2024</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CMS0000043</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>22.02.2024</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
         <v>1500</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Robo Test1</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3">
         <v>40001</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>1500</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>329</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Document 1800000443 was posted in company code 3000</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1800000443</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3">
         <v>2024</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CMS0000043</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>22.02.2024</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
         <v>2500</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Robo Test2</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
         <v>40001</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>2500</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>329</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Document 1800000444 was posted in company code 3000</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1800000444</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4">
         <v>2024</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pushing the variable file
</commit_message>
<xml_diff>
--- a/Tests/Resource/invoice.xlsx
+++ b/Tests/Resource/invoice.xlsx
@@ -1,104 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://beeceeyes-my.sharepoint.com/personal/brindha_m_basiscloudsolutions_com/Documents/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_5419CAB81A5FCACFE41724145073A63A9674775A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C419A51D-D3AC-476A-94F5-D0B08AEFC087}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="INPUT" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INPUT" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
-  <si>
-    <t xml:space="preserve"> Customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Invoice Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amount</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>G/L Account</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amount in doc. curr.</t>
-  </si>
-  <si>
-    <t>Cost Center</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
-    <t>Document</t>
-  </si>
-  <si>
-    <t>Company Code</t>
-  </si>
-  <si>
-    <t>Fiscal Year</t>
-  </si>
-  <si>
-    <t>CMS0000043</t>
-  </si>
-  <si>
-    <t>04.03.2024</t>
-  </si>
-  <si>
-    <t>Robo Test</t>
-  </si>
-  <si>
-    <t>Robo Test1</t>
-  </si>
-  <si>
-    <t>Robo Test2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -117,24 +46,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -454,152 +442,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" customWidth="1"/>
-    <col min="7" max="7" width="11.26953125" customWidth="1"/>
-    <col min="8" max="8" width="48.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" customWidth="1"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="25.6640625" customWidth="1" min="2" max="2"/>
+    <col width="15.44140625" customWidth="1" min="3" max="3"/>
+    <col width="15.6640625" customWidth="1" min="4" max="4"/>
+    <col width="15.5546875" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="17.6640625" customWidth="1" min="7" max="7"/>
+    <col width="54.5546875" customWidth="1" min="8" max="8"/>
+    <col width="26.5546875" customWidth="1" min="9" max="9"/>
+    <col width="27.44140625" customWidth="1" min="10" max="10"/>
+    <col width="13.109375" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Customer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Invoice Date</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Amount</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>G/L Account</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Amount in doc. curr.</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Cost Center</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Output</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Document</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Company Code</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Fiscal Year</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CMS0000043</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>05.03.2024</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1000</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Robo Test</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>40001</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>1000</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>329</v>
       </c>
-      <c r="K2">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Document 1800000518 was posted in company code 3000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1800000518</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CMS0000043</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>05.03.2024</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>1500</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Robo Test1</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>40001</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>1500</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>329</v>
       </c>
-      <c r="K3">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Document 1800000519 was posted in company code 3000</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1800000519</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
         <v>2024</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CMS0000043</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>05.03.2024</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>2500</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Robo Test2</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>40001</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>2500</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>329</v>
       </c>
-      <c r="K4">
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Document 1800000520 was posted in company code 3000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1800000520</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>